<commit_message>
Add MINGAS4 technology to FI_Process table
</commit_message>
<xml_diff>
--- a/VT_REG_PRI_V04.xlsx
+++ b/VT_REG_PRI_V04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA_2\Veda_models\demos004_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718F207-D7B3-4B0D-9CCA-DA65B35142A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06BF976-549C-46C8-933C-4D425253888F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="901" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8382,7 +8382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="219">
   <si>
     <t>CommName</t>
   </si>
@@ -9037,6 +9037,9 @@
   <si>
     <t>Reference Energy System</t>
   </si>
+  <si>
+    <t>MINGAS4</t>
+  </si>
 </sst>
 </file>
 
@@ -9651,7 +9654,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10051,6 +10054,7 @@
     <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -18501,8 +18505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19029,6 +19033,19 @@
       <c r="F16" s="16"/>
       <c r="G16" s="15"/>
       <c r="I16" s="23"/>
+      <c r="K16" s="227" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="227" t="s">
+        <v>218</v>
+      </c>
+      <c r="N16" s="216" t="str">
+        <f>"Domestic Supply of "&amp;$D$2&amp; " Step "&amp;RIGHT(M16,1)</f>
+        <v>Domestic Supply of Natural Gas Step 4</v>
+      </c>
+      <c r="O16" s="227" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="17" spans="2:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F17" s="16"/>

</xml_diff>

<commit_message>
Add data to MINGAS4 definition
</commit_message>
<xml_diff>
--- a/VT_REG_PRI_V04.xlsx
+++ b/VT_REG_PRI_V04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA_2\Veda_models\demos004_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06BF976-549C-46C8-933C-4D425253888F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7575F9BD-18B7-4B79-AA25-7714DB004321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="901" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18505,8 +18505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19027,12 +19027,26 @@
       <c r="T15"/>
     </row>
     <row r="16" spans="2:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="16"/>
+      <c r="B16" s="16" t="str">
+        <f>M16</f>
+        <v>MINGAS4</v>
+      </c>
       <c r="C16" s="16"/>
+      <c r="D16" s="16" t="str">
+        <f>$M$5</f>
+        <v>GAS</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="15"/>
-      <c r="I16" s="23"/>
+      <c r="G16" s="133">
+        <v>25000</v>
+      </c>
+      <c r="H16" s="135">
+        <v>5.4</v>
+      </c>
+      <c r="I16" s="133">
+        <v>2000</v>
+      </c>
       <c r="K16" s="227" t="s">
         <v>63</v>
       </c>

</xml_diff>